<commit_message>
Clear before big update
</commit_message>
<xml_diff>
--- a/Images/Style_Function_table_style_cells.xlsx
+++ b/Images/Style_Function_table_style_cells.xlsx
@@ -846,7 +846,6 @@
       <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="F7"/>
       <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
@@ -939,14 +938,12 @@
       <c r="B11" t="s">
         <v>55</v>
       </c>
-      <c r="C11"/>
       <c r="D11">
         <v>1800000</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="F11"/>
       <c r="G11" t="s">
         <v>57</v>
       </c>
@@ -961,7 +958,6 @@
       <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="C12"/>
       <c r="D12">
         <v>8250000</v>
       </c>
@@ -1020,7 +1016,6 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14"/>
       <c r="G14" t="s">
         <v>74</v>
       </c>

</xml_diff>